<commit_message>
Building the master branch
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -118,10 +118,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>

</xml_diff>